<commit_message>
Adjusted plotting code to plots for thesis
</commit_message>
<xml_diff>
--- a/1.3/Results.xlsx
+++ b/1.3/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie\Desktop\FYP\13\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie\Desktop\FYP\1.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,9 +35,6 @@
     <t>Avg</t>
   </si>
   <si>
-    <t>Hidden Setting</t>
-  </si>
-  <si>
     <t>50-5</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>100-50-20-5</t>
+  </si>
+  <si>
+    <t>Size of Hidden Layers</t>
   </si>
 </sst>
 </file>
@@ -411,17 +411,17 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -449,7 +449,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1.08E-4</v>
@@ -463,7 +463,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1.07E-4</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>1.0900000000000001E-4</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1.07E-4</v>
@@ -505,7 +505,7 @@
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>1.0900000000000001E-4</v>

</xml_diff>